<commit_message>
Progress on handl;ing intersections
</commit_message>
<xml_diff>
--- a/James/Parking Grid.xlsx
+++ b/James/Parking Grid.xlsx
@@ -204,7 +204,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -229,18 +229,18 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -274,10 +274,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -388,9 +384,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>475920</xdr:colOff>
+      <xdr:colOff>475560</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>342720</xdr:rowOff>
+      <xdr:rowOff>342360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -403,8 +399,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11114280" y="1472040"/>
-          <a:ext cx="4091040" cy="2802960"/>
+          <a:off x="11112480" y="1472040"/>
+          <a:ext cx="4086720" cy="2802600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -425,9 +421,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>614520</xdr:colOff>
+      <xdr:colOff>614160</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>507240</xdr:rowOff>
+      <xdr:rowOff>506880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -436,8 +432,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1848240" y="4946400"/>
-          <a:ext cx="1219680" cy="1015200"/>
+          <a:off x="1846800" y="4946400"/>
+          <a:ext cx="1219680" cy="1014840"/>
         </a:xfrm>
         <a:prstGeom prst="pie">
           <a:avLst>
@@ -445,7 +441,10 @@
             <a:gd name="adj2" fmla="val 10765624"/>
           </a:avLst>
         </a:prstGeom>
-        <a:ln/>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -473,9 +472,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>9000</xdr:colOff>
+      <xdr:colOff>8640</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>490680</xdr:rowOff>
+      <xdr:rowOff>490320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -484,8 +483,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8600400" y="4933080"/>
-          <a:ext cx="1238400" cy="1011960"/>
+          <a:off x="8598960" y="4933080"/>
+          <a:ext cx="1238040" cy="1011600"/>
         </a:xfrm>
         <a:prstGeom prst="pie">
           <a:avLst>
@@ -493,7 +492,10 @@
             <a:gd name="adj2" fmla="val 5662226"/>
           </a:avLst>
         </a:prstGeom>
-        <a:ln/>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -521,9 +523,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>28440</xdr:colOff>
+      <xdr:colOff>28080</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>495000</xdr:rowOff>
+      <xdr:rowOff>494640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -532,13 +534,16 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8886240" y="888120"/>
-          <a:ext cx="357120" cy="495000"/>
+          <a:off x="8884800" y="888120"/>
+          <a:ext cx="357120" cy="494640"/>
         </a:xfrm>
         <a:prstGeom prst="rtTriangle">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln/>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -568,7 +573,7 @@
   <dimension ref="C2:Q14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
+      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -636,7 +641,7 @@
       <c r="M4" s="6"/>
       <c r="N4" s="7"/>
       <c r="O4" s="8"/>
-      <c r="P4" s="6"/>
+      <c r="P4" s="8"/>
       <c r="Q4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -676,35 +681,35 @@
     <row r="7" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C7" s="16"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="19"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="18"/>
       <c r="G7" s="17"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="19"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="18"/>
       <c r="J7" s="17"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="19"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="18"/>
       <c r="M7" s="17"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="19"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="18"/>
       <c r="P7" s="17"/>
-      <c r="Q7" s="18"/>
+      <c r="Q7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C8" s="20"/>
-      <c r="D8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="18"/>
       <c r="E8" s="7"/>
       <c r="F8" s="17"/>
-      <c r="G8" s="19"/>
+      <c r="G8" s="18"/>
       <c r="H8" s="7"/>
       <c r="I8" s="17"/>
-      <c r="J8" s="19"/>
+      <c r="J8" s="18"/>
       <c r="K8" s="7"/>
       <c r="L8" s="17"/>
-      <c r="M8" s="19"/>
+      <c r="M8" s="18"/>
       <c r="N8" s="7"/>
       <c r="O8" s="17"/>
-      <c r="P8" s="19"/>
+      <c r="P8" s="18"/>
       <c r="Q8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -714,25 +719,25 @@
       <c r="F9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="19"/>
+      <c r="G9" s="18"/>
       <c r="H9" s="4"/>
       <c r="I9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="19"/>
+      <c r="J9" s="18"/>
       <c r="K9" s="4"/>
       <c r="L9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M9" s="19"/>
+      <c r="M9" s="18"/>
       <c r="N9" s="4"/>
       <c r="O9" s="15"/>
       <c r="P9" s="14"/>
       <c r="Q9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C10" s="20"/>
-      <c r="D10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="18"/>
       <c r="E10" s="7"/>
       <c r="F10" s="8"/>
       <c r="G10" s="6"/>
@@ -744,7 +749,7 @@
       <c r="M10" s="6"/>
       <c r="N10" s="7"/>
       <c r="O10" s="17"/>
-      <c r="P10" s="19"/>
+      <c r="P10" s="18"/>
       <c r="Q10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -771,8 +776,8 @@
       <c r="F12" s="15"/>
       <c r="G12" s="17"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="18"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="6"/>
       <c r="K12" s="4"/>
       <c r="L12" s="15"/>
       <c r="M12" s="17"/>
@@ -782,20 +787,20 @@
       <c r="Q12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C13" s="20"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="18"/>
       <c r="J13" s="17"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="17"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="6"/>
       <c r="Q13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -805,10 +810,10 @@
       <c r="F14" s="12"/>
       <c r="G14" s="17"/>
       <c r="H14" s="11"/>
-      <c r="I14" s="23" t="s">
+      <c r="I14" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="J14" s="24"/>
+      <c r="J14" s="23"/>
       <c r="K14" s="11"/>
       <c r="L14" s="12"/>
       <c r="M14" s="17"/>

</xml_diff>